<commit_message>
Adding commits for LCIA
</commit_message>
<xml_diff>
--- a/LCA/ASPEN-MASS-FLOWS.xlsx
+++ b/LCA/ASPEN-MASS-FLOWS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t xml:space="preserve">Mass Flows</t>
   </si>
@@ -85,10 +85,7 @@
     <t xml:space="preserve">CO2</t>
   </si>
   <si>
-    <t xml:space="preserve">cyclohexane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toluene</t>
+    <t xml:space="preserve">hexane</t>
   </si>
   <si>
     <t xml:space="preserve">Ενεργειακές απαιτήσεις</t>
@@ -352,7 +349,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -615,8 +612,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -769,38 +766,38 @@
       </c>
       <c r="I9" s="1" t="n">
         <f aca="false">D10/F16</f>
-        <v>0.0431191720463162</v>
+        <v>0.0441541141510401</v>
       </c>
       <c r="L9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>84.16</v>
+        <v>86.18</v>
       </c>
       <c r="I10" s="1"/>
       <c r="K10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="n">
         <f aca="false">SUM(B8:D11)</f>
-        <v>4204.26</v>
+        <v>4206.28</v>
       </c>
       <c r="H11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,42 +809,42 @@
         <v>2.02918331796291</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="L12" s="1" t="n">
         <f aca="false">B29/$F$16</f>
         <v>5.18455286812173</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="H13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="n">
+        <v>6.18370048160672</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>6.18370048160672</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <f aca="false">B30/$F$16</f>
         <v>0.0264786648222154</v>
       </c>
@@ -860,16 +857,15 @@
         <v>0.942</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1769.06</v>
+        <v>1768.75</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>124.236</v>
-      </c>
-      <c r="H14" s="0"/>
-      <c r="K14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="0" t="n">
+        <v>124.54</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="1" t="n">
         <f aca="false">B31/$F$16</f>
         <v>1.04795060969362</v>
       </c>
@@ -885,35 +881,35 @@
         <v>0.02</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="1" t="n">
         <f aca="false">B32/$F$16</f>
         <v>1.73151449943642</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <f aca="false">L14+L15</f>
         <v>2.77946510913003</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>2.0904</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>57.56</v>
+      <c r="C16" s="1" t="n">
+        <v>60.57</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>177.996</v>
+        <v>175.906</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>1951.8</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -921,10 +917,10 @@
       </c>
       <c r="I16" s="1" t="n">
         <f aca="false">SUM(B14:D14)/F16</f>
-        <v>0.970508248795983</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>39</v>
+        <v>0.970505174710524</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,10 +928,10 @@
         <v>21</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>1.75</v>
+        <v>1.11</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>82.4135</v>
+        <v>85.06</v>
       </c>
       <c r="E17" s="1"/>
       <c r="H17" s="1" t="s">
@@ -946,47 +942,45 @@
         <v>0.00116815247463879</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="L17" s="1" t="n">
         <f aca="false">B34/$F$16</f>
         <v>0.199793561840353</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.0035</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>0.1338</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>0.0005</v>
-      </c>
+        <v>1.89</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="n">
-        <v>32.32</v>
+        <v>32.634</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="1" t="n">
         <f aca="false">SUM(B16:D16)/F16</f>
-        <v>0.121757557126755</v>
+        <v>0.122228916897223</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L18" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="L18" s="1" t="n">
         <f aca="false">B35/$F$16</f>
         <v>1.00348677118557</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -994,19 +988,19 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="n">
         <f aca="false">SUM(B14:E18)</f>
-        <v>2250.7857</v>
+        <v>2255.7759</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">F16/F16</f>
         <v>1</v>
       </c>
-      <c r="K19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="0" t="n">
+      <c r="K19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" s="1" t="n">
         <f aca="false">B36/$F$16</f>
         <v>0.627994671585203</v>
       </c>
@@ -1017,57 +1011,54 @@
       </c>
       <c r="I20" s="1" t="n">
         <f aca="false">SUM(C17:E17)/F16</f>
-        <v>0.0431209652628343</v>
+        <v>0.0441489906752741</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L20" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="L20" s="1" t="n">
         <f aca="false">B37/$F$16</f>
         <v>1.29836048775489</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <f aca="false">L19+L20</f>
         <v>1.9263551593401</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="1" t="n">
         <f aca="false">SUM(B18:E18)/F16</f>
-        <v>0.0166296751716364</v>
-      </c>
-      <c r="K21" s="0"/>
+        <v>0.0176900809509171</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="0"/>
-      <c r="K22" s="0"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1465.15</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>21067.3</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I24" s="1" t="n">
         <f aca="false">B23/$F$16</f>
@@ -1076,13 +1067,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>90347.9</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I25" s="1" t="n">
         <f aca="false">B24/$F$16</f>
@@ -1091,7 +1082,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I26" s="1" t="n">
         <f aca="false">B25/$F$16</f>
@@ -1100,111 +1091,100 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="0"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="0"/>
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <f aca="false">0.942/F16+B15/F16+B16/F16+B18/F16</f>
+        <v>0.00271334153089456</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="n">
         <f aca="false">47.732124*(237-25)</f>
         <v>10119.210288</v>
       </c>
-      <c r="H29" s="0"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B30" s="1" t="n">
         <f aca="false">4.698278*(248-237)</f>
         <v>51.681058</v>
       </c>
-      <c r="H30" s="0"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B31" s="1" t="n">
         <f aca="false">2045.39</f>
         <v>2045.39</v>
       </c>
-      <c r="H31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B32" s="1" t="n">
         <v>3379.57</v>
       </c>
-      <c r="H32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="0"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B34" s="1" t="n">
         <f aca="false">4.698278*(238-155)</f>
         <v>389.957074</v>
       </c>
-      <c r="H34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B35" s="1" t="n">
         <f aca="false">15.066196*(155-25)</f>
         <v>1958.60548</v>
       </c>
-      <c r="H35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>1225.72</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>1225.72</v>
-      </c>
-      <c r="H36" s="0"/>
-      <c r="K36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>2534.14</v>
       </c>
-      <c r="H37" s="0"/>
-      <c r="K37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="H38" s="0"/>
-      <c r="K38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="H39" s="0"/>
-      <c r="K39" s="0"/>
-    </row>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Commiting the final changes of the second progress report
</commit_message>
<xml_diff>
--- a/LCA/ASPEN-MASS-FLOWS.xlsx
+++ b/LCA/ASPEN-MASS-FLOWS.xlsx
@@ -613,7 +613,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1124,6 +1124,10 @@
         <f aca="false">4.698278*(248-237)</f>
         <v>51.681058</v>
       </c>
+      <c r="H30" s="1" t="n">
+        <f aca="false">(20931.6+3808+1175+15)/F16</f>
+        <v>13.2849677221027</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>

</xml_diff>